<commit_message>
Ignore changes in data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\intento_programa_balances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\internado\balance_neonatologia_intermedios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377E632-09A5-4E07-BB1F-A8E77BFE92BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF99FD-6BBB-4756-8ED7-82FFDF012AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{850AEF08-BD2C-4EEB-8914-E70EBF671138}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{850AEF08-BD2C-4EEB-8914-E70EBF671138}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>paciente</t>
   </si>
@@ -67,7 +67,10 @@
     <t>egreso_deposiciones</t>
   </si>
   <si>
-    <t>larico</t>
+    <t>sandoval</t>
+  </si>
+  <si>
+    <t>corbacho</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57AE89B-F1A1-4D23-A164-B6AFA34C37D1}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +555,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>45107</v>
@@ -590,7 +593,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>45108</v>
@@ -628,7 +631,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>45109</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>45110</v>
@@ -676,6 +679,58 @@
       </c>
       <c r="D7">
         <v>1650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45114</v>
+      </c>
+      <c r="C8">
+        <v>1670</v>
+      </c>
+      <c r="D8">
+        <v>1632</v>
+      </c>
+      <c r="E8">
+        <v>138.1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <v>204</v>
+      </c>
+      <c r="J8">
+        <v>95</v>
+      </c>
+      <c r="K8">
+        <v>60</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45115</v>
+      </c>
+      <c r="C9">
+        <v>1670</v>
+      </c>
+      <c r="D9">
+        <v>1598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>